<commit_message>
[Modified]: Edit ManageUserInfo AD: edit flows and remove some processes
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Dữ Liệu/temp/Project.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Dữ Liệu/temp/Project.xlsx
@@ -117,7 +117,7 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>Duy nhất, theo định dạng "US00001"</t>
+    <t>Theo định dạng "US00001"</t>
   </si>
   <si>
     <t>"US00001"</t>
@@ -130,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -150,6 +150,10 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -202,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -224,10 +228,13 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf quotePrefix="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,7 +645,7 @@
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -684,7 +691,7 @@
       <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -721,13 +728,13 @@
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="4" t="s">

</xml_diff>